<commit_message>
MAINTANANCE Sync with develop [SG, DK]
</commit_message>
<xml_diff>
--- a/PairProgramming/PairingMatrix_Team_22.xlsx
+++ b/PairProgramming/PairingMatrix_Team_22.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo-t440s-LIANA\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6A067BE2-95DE-4BA1-8E79-4C6DFB0AD345}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C12EC96C-D70E-42F1-9495-53462B492A6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="14">
   <si>
     <t>Number of minutes the two members did physically co-located ping pong pair programming.</t>
   </si>
@@ -71,6 +71,9 @@
   </si>
   <si>
     <t xml:space="preserve">Riccardo Baljak </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                   </t>
   </si>
 </sst>
 </file>
@@ -489,10 +492,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I26"/>
+  <dimension ref="A1:N30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -805,12 +808,18 @@
         <v>5</v>
       </c>
       <c r="B15" s="3"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
+      <c r="E15" s="4">
+        <v>660</v>
+      </c>
+      <c r="F15" s="4">
+        <v>150</v>
+      </c>
       <c r="G15" s="4">
         <v>300</v>
       </c>
-      <c r="H15" s="4"/>
+      <c r="H15" s="4">
+        <v>90</v>
+      </c>
       <c r="I15" s="4">
         <v>60</v>
       </c>
@@ -823,16 +832,20 @@
         <f>C15</f>
         <v>0</v>
       </c>
-      <c r="C16" s="3"/>
+      <c r="C16" s="3">
+        <v>60</v>
+      </c>
       <c r="E16" s="4"/>
       <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="G16" s="4">
+        <v>660</v>
+      </c>
       <c r="H16" s="4">
-        <v>510</v>
+        <v>660</v>
       </c>
       <c r="I16" s="4"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -845,23 +858,27 @@
         <v>0</v>
       </c>
       <c r="D17" s="3"/>
-      <c r="E17" s="4"/>
+      <c r="E17" s="4">
+        <v>150</v>
+      </c>
       <c r="F17" s="4"/>
       <c r="G17" s="4">
-        <v>270</v>
-      </c>
-      <c r="H17" s="4"/>
+        <v>330</v>
+      </c>
+      <c r="H17" s="4">
+        <v>450</v>
+      </c>
       <c r="I17" s="4">
         <v>430</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="5">
         <f>E15</f>
-        <v>0</v>
+        <v>660</v>
       </c>
       <c r="C18" s="5">
         <f>E16</f>
@@ -869,23 +886,23 @@
       </c>
       <c r="D18" s="5">
         <f>E17</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="4">
-        <v>570</v>
+        <v>600</v>
       </c>
       <c r="G18" s="4"/>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
     </row>
-    <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B19" s="5">
         <f>F15</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="C19" s="5">
         <f>F16</f>
@@ -897,14 +914,16 @@
       </c>
       <c r="E19" s="5">
         <f>F18</f>
-        <v>570</v>
+        <v>600</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="4"/>
       <c r="H19" s="4"/>
-      <c r="I19" s="4"/>
-    </row>
-    <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I19" s="4">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>10</v>
       </c>
@@ -914,11 +933,11 @@
       </c>
       <c r="C20" s="5">
         <f>G16</f>
-        <v>0</v>
+        <v>660</v>
       </c>
       <c r="D20" s="5">
         <f>G17</f>
-        <v>270</v>
+        <v>330</v>
       </c>
       <c r="E20" s="5">
         <f>G18</f>
@@ -930,23 +949,25 @@
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="4"/>
-      <c r="I20" s="4"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="I20" s="4">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B21" s="5">
         <f>H15</f>
-        <v>0</v>
+        <v>90</v>
       </c>
       <c r="C21" s="5">
         <f>H16</f>
-        <v>510</v>
+        <v>660</v>
       </c>
       <c r="D21" s="5">
         <f>H17</f>
-        <v>0</v>
+        <v>450</v>
       </c>
       <c r="E21" s="5">
         <f>H18</f>
@@ -963,7 +984,7 @@
       <c r="H21" s="3"/>
       <c r="I21" s="4"/>
     </row>
-    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
@@ -985,11 +1006,11 @@
       </c>
       <c r="F22" s="5">
         <f>I19</f>
-        <v>0</v>
+        <v>660</v>
       </c>
       <c r="G22" s="5">
         <f>I20</f>
-        <v>0</v>
+        <v>150</v>
       </c>
       <c r="H22" s="5">
         <f>I21</f>
@@ -999,118 +1020,123 @@
         <v>150</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B23" s="8">
-        <f>SUM(B15:B22)</f>
-        <v>360</v>
+        <f t="shared" ref="B23:I23" si="1">SUM(B15:B22)</f>
+        <v>1260</v>
       </c>
       <c r="C23" s="8">
-        <f>SUM(C15:C22)</f>
-        <v>510</v>
+        <f t="shared" si="1"/>
+        <v>1380</v>
       </c>
       <c r="D23" s="8">
-        <f>SUM(D15:D22)</f>
-        <v>700</v>
+        <f t="shared" si="1"/>
+        <v>1360</v>
       </c>
       <c r="E23" s="8">
-        <f>SUM(E15:E22)</f>
-        <v>570</v>
+        <f t="shared" si="1"/>
+        <v>1410</v>
       </c>
       <c r="F23" s="8">
-        <f>SUM(F15:F22)</f>
-        <v>570</v>
+        <f t="shared" si="1"/>
+        <v>1410</v>
       </c>
       <c r="G23" s="8">
-        <f>SUM(G15:G22)</f>
-        <v>570</v>
+        <f t="shared" si="1"/>
+        <v>1440</v>
       </c>
       <c r="H23" s="8">
-        <f>SUM(H15:H22)</f>
-        <v>510</v>
+        <f t="shared" si="1"/>
+        <v>1200</v>
       </c>
       <c r="I23" s="8">
-        <f>SUM(I15:I22)</f>
-        <v>640</v>
-      </c>
-    </row>
-    <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="9" t="s">
         <v>3</v>
       </c>
       <c r="B25" s="10">
-        <f t="shared" ref="B25:I25" si="1">B11+B23</f>
-        <v>360</v>
+        <f t="shared" ref="B25:I25" si="2">B11+B23</f>
+        <v>1260</v>
       </c>
       <c r="C25" s="10">
         <f>C11+C23</f>
-        <v>510</v>
+        <v>1380</v>
       </c>
       <c r="D25" s="10">
-        <f t="shared" si="1"/>
-        <v>700</v>
+        <f t="shared" si="2"/>
+        <v>1360</v>
       </c>
       <c r="E25" s="10">
-        <f t="shared" si="1"/>
-        <v>570</v>
+        <f t="shared" si="2"/>
+        <v>1410</v>
       </c>
       <c r="F25" s="10">
-        <f t="shared" si="1"/>
-        <v>570</v>
+        <f t="shared" si="2"/>
+        <v>1410</v>
       </c>
       <c r="G25" s="10">
-        <f t="shared" si="1"/>
-        <v>570</v>
+        <f t="shared" si="2"/>
+        <v>1440</v>
       </c>
       <c r="H25" s="10">
-        <f t="shared" si="1"/>
-        <v>510</v>
+        <f t="shared" si="2"/>
+        <v>1200</v>
       </c>
       <c r="I25" s="10">
-        <f t="shared" si="1"/>
-        <v>640</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+        <f t="shared" si="2"/>
+        <v>1450</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>4</v>
       </c>
       <c r="B26" s="12">
-        <f t="shared" ref="B26:I26" si="2">B25/60/24</f>
-        <v>0.25</v>
+        <f t="shared" ref="B26:I26" si="3">B25/60/24</f>
+        <v>0.875</v>
       </c>
       <c r="C26" s="12">
         <f>C25/60/24</f>
-        <v>0.35416666666666669</v>
+        <v>0.95833333333333337</v>
       </c>
       <c r="D26" s="12">
-        <f t="shared" si="2"/>
-        <v>0.4861111111111111</v>
+        <f t="shared" si="3"/>
+        <v>0.94444444444444453</v>
       </c>
       <c r="E26" s="12">
-        <f t="shared" si="2"/>
-        <v>0.39583333333333331</v>
+        <f t="shared" si="3"/>
+        <v>0.97916666666666663</v>
       </c>
       <c r="F26" s="12">
-        <f t="shared" si="2"/>
-        <v>0.39583333333333331</v>
+        <f t="shared" si="3"/>
+        <v>0.97916666666666663</v>
       </c>
       <c r="G26" s="12">
-        <f t="shared" si="2"/>
-        <v>0.39583333333333331</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="H26" s="12">
-        <f t="shared" si="2"/>
-        <v>0.35416666666666669</v>
+        <f t="shared" si="3"/>
+        <v>0.83333333333333337</v>
       </c>
       <c r="I26" s="12">
-        <f t="shared" si="2"/>
-        <v>0.44444444444444442</v>
+        <f t="shared" si="3"/>
+        <v>1.0069444444444444</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="N30" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>